<commit_message>
Added Divisional Round Forecasts
</commit_message>
<xml_diff>
--- a/Playoff Predictions/Weekwc_matrix.xlsx
+++ b/Playoff Predictions/Weekwc_matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Matchups" sheetId="1" r:id="rId1"/>
@@ -660,6 +660,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -684,7 +685,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5517,8 +5517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5571,10 +5571,10 @@
       <c r="E2" s="36"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="42"/>
+      <c r="I2" s="43"/>
       <c r="J2" s="36"/>
       <c r="K2" s="36"/>
       <c r="L2" s="36"/>
@@ -5591,10 +5591,10 @@
       <c r="E3" s="36"/>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
-      <c r="H3" s="45" t="s">
+      <c r="H3" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="46"/>
+      <c r="I3" s="47"/>
       <c r="J3" s="36"/>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
@@ -5611,10 +5611,10 @@
       <c r="E4" s="36"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="44"/>
+      <c r="I4" s="45"/>
       <c r="J4" s="36"/>
       <c r="K4" s="36"/>
       <c r="L4" s="36"/>
@@ -5631,10 +5631,10 @@
       <c r="E5" s="36"/>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="48"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="36"/>
       <c r="K5" s="36"/>
       <c r="L5" s="36"/>
@@ -10941,7 +10941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -10974,7 +10974,7 @@
       <c r="E2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="41">
         <f>B2*B8</f>
         <v>0.13614613897104683</v>
       </c>

</xml_diff>